<commit_message>
POM registration/assert with all my profile fields
</commit_message>
<xml_diff>
--- a/projectInputData.xlsx
+++ b/projectInputData.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="4455" activeTab="1" xr2:uid="{2D209322-F75F-40A7-B668-BC813A9CDAB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="4455" firstSheet="1" activeTab="1" xr2:uid="{2D209322-F75F-40A7-B668-BC813A9CDAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="loginInfo" sheetId="1" r:id="rId1"/>
     <sheet name="registrationInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="verifyRegistration" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>kisulea</t>
   </si>
@@ -102,9 +104,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>JohnSmith@gmail.com</t>
-  </si>
-  <si>
     <t>78 Main st.</t>
   </si>
   <si>
@@ -123,9 +122,6 @@
     <t>Erny</t>
   </si>
   <si>
-    <t>AlexErny@gmail.com</t>
-  </si>
-  <si>
     <t>435 Los G St.</t>
   </si>
   <si>
@@ -153,7 +149,52 @@
     <t>password</t>
   </si>
   <si>
-    <t>MashaRey21@yahoo.com</t>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Apt.2</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>MashaRey12345@yahoo.com</t>
+  </si>
+  <si>
+    <t>JohnSmith12@gmail.com</t>
+  </si>
+  <si>
+    <t>AlexErny21@gmail.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>(789) 876-7877</t>
+  </si>
+  <si>
+    <t>(789) 898-7890</t>
+  </si>
+  <si>
+    <t>(676) 567-8767</t>
+  </si>
+  <si>
+    <t>alexerny345677@gmail.com</t>
+  </si>
+  <si>
+    <t>johnjmith345677@gmail.com</t>
+  </si>
+  <si>
+    <t>masharey915677@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -567,25 +608,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE168D-8980-4823-8768-3A5CEB9FA94C}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -596,34 +638,37 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -634,34 +679,37 @@
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="E2">
-        <v>7898767877</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
       <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>87678</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -672,66 +720,75 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="E3">
-        <v>7898987890</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3">
+        <v>98098</v>
+      </c>
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="J3">
-        <v>98098</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="E4">
-        <v>6765678767</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>76890</v>
+      </c>
+      <c r="L4" t="s">
         <v>36</v>
       </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4">
-        <v>76890</v>
-      </c>
-      <c r="K4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
+      <c r="M4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -742,4 +799,82 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C46892-8ADB-49AB-A869-38566057FB56}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{8B820E71-2D4A-43AD-A5E6-FD482B13A568}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178435F0-B8E4-4030-8F8A-8B6136DE29A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
POM ChangePassword negative test and error messages
</commit_message>
<xml_diff>
--- a/projectInputData.xlsx
+++ b/projectInputData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="4455" firstSheet="1" activeTab="1" xr2:uid="{2D209322-F75F-40A7-B668-BC813A9CDAB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="4455" activeTab="3" xr2:uid="{2D209322-F75F-40A7-B668-BC813A9CDAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="loginInfo" sheetId="1" r:id="rId1"/>
     <sheet name="registrationInfo" sheetId="2" r:id="rId2"/>
     <sheet name="verifyRegistration" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="changePasswordNegative" sheetId="4" r:id="rId4"/>
+    <sheet name="userPass" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>kisulea</t>
   </si>
   <si>
-    <t>buquxahu@cars2.club</t>
-  </si>
-  <si>
     <t>filllipa12345@yahoo.com</t>
   </si>
   <si>
@@ -195,6 +193,45 @@
   </si>
   <si>
     <t>masharey915677@yahoo.com</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confirmNewPassword</t>
+  </si>
+  <si>
+    <t>milla12345</t>
+  </si>
+  <si>
+    <t>milla123</t>
+  </si>
+  <si>
+    <t>1234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890</t>
+  </si>
+  <si>
+    <t>phillipa</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>The passwords do not match.</t>
+  </si>
+  <si>
+    <t>Current password is wrong.</t>
+  </si>
+  <si>
+    <t>This value is too short. It should have 6 characters or more.</t>
+  </si>
+  <si>
+    <t>This value is too long. It should have 255 characters or fewer.</t>
   </si>
 </sst>
 </file>
@@ -563,7 +600,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,10 +611,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,24 +622,23 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{66353DBB-4E37-4F9C-9426-07C3AE1994AF}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0C1FF720-FADA-4E39-AB65-51A37FD4D7BB}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0C1FF720-FADA-4E39-AB65-51A37FD4D7BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -610,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE168D-8980-4823-8768-3A5CEB9FA94C}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -629,166 +665,166 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
       <c r="K2">
         <v>87678</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
       </c>
       <c r="K3">
         <v>98098</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
       <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
         <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
       </c>
       <c r="K4">
         <v>76890</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -805,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C46892-8ADB-49AB-A869-38566057FB56}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,46 +853,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -869,12 +905,130 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178435F0-B8E4-4030-8F8A-8B6136DE29A0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13C4226-1907-4CD6-8BB9-1853A233F1E8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7BC2CBA2-DA22-477B-868F-EB1ACF54BA0E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>